<commit_message>
Updated till 25 Aug 2025
</commit_message>
<xml_diff>
--- a/2025_Pilot_Study/Field_Data/Field_Data.xlsx
+++ b/2025_Pilot_Study/Field_Data/Field_Data.xlsx
@@ -398,7 +398,7 @@
   <dimension ref="A1:J136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,16 +1001,45 @@
         <v>10</v>
       </c>
       <c r="B26" s="2">
-        <v>45880</v>
-      </c>
-      <c r="C26" s="3"/>
+        <v>45882</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.55833333333333335</v>
+      </c>
+      <c r="D26">
+        <v>29</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="2">
-        <v>45880</v>
+        <v>45882</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.56111111111111112</v>
+      </c>
+      <c r="D27">
+        <v>29.8</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1018,7 +1047,22 @@
         <v>12</v>
       </c>
       <c r="B28" s="2">
-        <v>45880</v>
+        <v>45882</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="D28">
+        <v>28.9</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -1026,7 +1070,22 @@
         <v>13</v>
       </c>
       <c r="B29" s="2">
-        <v>45880</v>
+        <v>45882</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="D29">
+        <v>29.9</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -1034,7 +1093,22 @@
         <v>14</v>
       </c>
       <c r="B30" s="2">
-        <v>45880</v>
+        <v>45882</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="D30">
+        <v>27.3</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -1042,7 +1116,22 @@
         <v>15</v>
       </c>
       <c r="B31" s="2">
-        <v>45880</v>
+        <v>45882</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.57222222222222219</v>
+      </c>
+      <c r="D31">
+        <v>29</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added 3 Sep data and updated graph
</commit_message>
<xml_diff>
--- a/2025_Pilot_Study/Field_Data/Field_Data.xlsx
+++ b/2025_Pilot_Study/Field_Data/Field_Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
   <si>
     <t>Plot</t>
   </si>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J136"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="E28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,28 +1273,142 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="2"/>
-      <c r="C38" s="3"/>
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="2">
+        <v>45903</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.50486111111111109</v>
+      </c>
+      <c r="D38">
+        <v>31.4</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
+      <c r="J38">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="2"/>
-      <c r="C39" s="3"/>
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="2">
+        <v>45903</v>
+      </c>
+      <c r="C39" s="3">
+        <v>0.50972222222222219</v>
+      </c>
+      <c r="D39">
+        <v>31.2</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <v>4</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="2"/>
-      <c r="C40" s="3"/>
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="2">
+        <v>45903</v>
+      </c>
+      <c r="C40" s="3">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D40">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="2"/>
-      <c r="C41" s="3"/>
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="2">
+        <v>45903</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.53055555555555556</v>
+      </c>
+      <c r="D41">
+        <v>31.5</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B42" s="2"/>
-      <c r="C42" s="3"/>
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="2">
+        <v>45903</v>
+      </c>
+      <c r="C42" s="3">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="D42">
+        <v>31.5</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B43" s="2"/>
-      <c r="C43" s="3"/>
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="2">
+        <v>45903</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.53611111111111109</v>
+      </c>
+      <c r="D43">
+        <v>31.5</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>3</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>

</xml_diff>